<commit_message>
GATE 2021 Syllabus Updated
Updated Syllabus
</commit_message>
<xml_diff>
--- a/Links/Subjects_Concepts_Links.xlsx
+++ b/Links/Subjects_Concepts_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GATE\GATE_CS_2021\Links\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739C76DC-F53F-4B27-B25F-2AC8F4E667AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F752D-27EF-4075-97C3-70C7A78B36D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Chapter</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>Main DAA Concepts</t>
+  </si>
+  <si>
+    <t>Topological Sorting</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qe_pQCh09yU</t>
   </si>
 </sst>
 </file>
@@ -192,10 +198,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -507,7 +513,7 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -518,7 +524,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -616,26 +622,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E58C2A-E329-4A0A-9EC8-C16EBCEDCA35}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -673,6 +680,14 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -680,8 +695,9 @@
     <hyperlink ref="C4" r:id="rId1" xr:uid="{0DFD4216-78D4-46B3-A129-7B7493D93BE4}"/>
     <hyperlink ref="C6" r:id="rId2" xr:uid="{CED834C9-83A6-41B6-A7CB-8109327D3FD8}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{F26F46A7-E3F5-4E80-895E-6517BF70CC48}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{6C4BBB97-CEC6-4AD7-9815-BC31AED02AD6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>